<commit_message>
Upload Ofner2017 (results distributions fit)
</commit_message>
<xml_diff>
--- a/stats_std_and_training.xlsx
+++ b/stats_std_and_training.xlsx
@@ -5,10 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Ofner2017" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Ofner2017_distributions" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="134">
   <si>
     <t xml:space="preserve">Recon quality</t>
   </si>
@@ -95,6 +96,333 @@
   </si>
   <si>
     <t xml:space="preserve">Case 2 (anche se non così marcato)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Distribution</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Average position (train)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Average position (test)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Average position (both)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Average error (train)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Average error (test)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Average error (both)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">genhyperbolic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">burr12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">burr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">norminvgauss</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mielke</t>
+  </si>
+  <si>
+    <t xml:space="preserve">johnsonsu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fisk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">exponnorm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nct</t>
+  </si>
+  <si>
+    <t xml:space="preserve">genlogistic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">alpha</t>
+  </si>
+  <si>
+    <t xml:space="preserve">f</t>
+  </si>
+  <si>
+    <t xml:space="preserve">invgamma</t>
+  </si>
+  <si>
+    <t xml:space="preserve">betaprime</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lognorm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fatiguelife</t>
+  </si>
+  <si>
+    <t xml:space="preserve">genextreme</t>
+  </si>
+  <si>
+    <t xml:space="preserve">exponweib</t>
+  </si>
+  <si>
+    <t xml:space="preserve">johnsonsb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">powerlognorm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">recipinvgauss</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hypsecant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">t</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ncf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">logistic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">invweibull</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gennorm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dweibull</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gengamma</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pearson3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dgamma</t>
+  </si>
+  <si>
+    <t xml:space="preserve">loglaplace</t>
+  </si>
+  <si>
+    <t xml:space="preserve">erlang</t>
+  </si>
+  <si>
+    <t xml:space="preserve">invgauss</t>
+  </si>
+  <si>
+    <t xml:space="preserve">skewnorm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">geninvgauss</t>
+  </si>
+  <si>
+    <t xml:space="preserve">beta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">chi2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">laplace</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tukeylambda</t>
+  </si>
+  <si>
+    <t xml:space="preserve">powernorm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ncx2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">moyal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">foldcauchy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">skewcauchy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nakagami</t>
+  </si>
+  <si>
+    <t xml:space="preserve">chi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cauchy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gamma</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kstwobign</t>
+  </si>
+  <si>
+    <t xml:space="preserve">maxwell</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rice</t>
+  </si>
+  <si>
+    <t xml:space="preserve">crystalball</t>
+  </si>
+  <si>
+    <t xml:space="preserve">norm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">foldnorm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">loggamma</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rayleigh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">genexpon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rdist</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kappa3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wald</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gibrat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">truncnorm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gompertz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">exponpow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">halfnorm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">halflogistic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gausshyper</t>
+  </si>
+  <si>
+    <t xml:space="preserve">halfgennorm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">genhalflogistic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cosine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">genpareto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">triang</t>
+  </si>
+  <si>
+    <t xml:space="preserve">halfcauchy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">levy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">expon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pareto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lomax</t>
+  </si>
+  <si>
+    <t xml:space="preserve">anglit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">truncpareto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reciprocal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kappa4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bradford</t>
+  </si>
+  <si>
+    <t xml:space="preserve">truncexpon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vonmises</t>
+  </si>
+  <si>
+    <t xml:space="preserve">semicircular</t>
+  </si>
+  <si>
+    <t xml:space="preserve">powerlaw</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wrapcauchy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">uniform</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ksone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">argus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">arcsine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">trapezoid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">jf</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> inf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">studentized</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gumbel</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> nan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">weibull</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kstwo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">truncweibull</t>
   </si>
 </sst>
 </file>
@@ -128,12 +456,24 @@
       <family val="0"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFBF00"/>
+        <bgColor rgb="FFFF9900"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor rgb="FF993300"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="16">
@@ -275,7 +615,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -372,6 +712,14 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -381,6 +729,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFBF00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -391,7 +799,7 @@
   </sheetPr>
   <dimension ref="A1:N32"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
@@ -1138,4 +1546,2544 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:G109"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="21.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="18.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="18.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="19.08"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>8.07</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>9.07</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>8.57</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <v>0.019</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <v>0.023</v>
+      </c>
+      <c r="G2" s="0" t="n">
+        <v>0.021</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>8.33</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>8.67</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>0.029</v>
+      </c>
+      <c r="F3" s="0" t="n">
+        <v>0.031</v>
+      </c>
+      <c r="G3" s="0" t="n">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>9.73</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>8.4</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>9.07</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>0.032</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <v>0.031</v>
+      </c>
+      <c r="G4" s="0" t="n">
+        <v>0.031</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>10.2</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>8.07</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>9.13</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>0.024</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <v>0.025</v>
+      </c>
+      <c r="G5" s="0" t="n">
+        <v>0.025</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>11.13</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>7.4</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>9.27</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>0.032</v>
+      </c>
+      <c r="F6" s="0" t="n">
+        <v>0.031</v>
+      </c>
+      <c r="G6" s="0" t="n">
+        <v>0.032</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>10.8</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>9.4</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>0.026</v>
+      </c>
+      <c r="F7" s="0" t="n">
+        <v>0.027</v>
+      </c>
+      <c r="G7" s="0" t="n">
+        <v>0.026</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>9.87</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>11.6</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <v>10.73</v>
+      </c>
+      <c r="E8" s="0" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="F8" s="0" t="n">
+        <v>0.035</v>
+      </c>
+      <c r="G8" s="0" t="n">
+        <v>0.032</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>11.73</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>10.4</v>
+      </c>
+      <c r="D9" s="0" t="n">
+        <v>11.07</v>
+      </c>
+      <c r="E9" s="0" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="F9" s="0" t="n">
+        <v>0.055</v>
+      </c>
+      <c r="G9" s="0" t="n">
+        <v>0.053</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>14.69</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>10.07</v>
+      </c>
+      <c r="D10" s="0" t="n">
+        <v>12.21</v>
+      </c>
+      <c r="E10" s="0" t="n">
+        <v>0.067</v>
+      </c>
+      <c r="F10" s="0" t="n">
+        <v>0.063</v>
+      </c>
+      <c r="G10" s="0" t="n">
+        <v>0.065</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <v>12.93</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>15.73</v>
+      </c>
+      <c r="D11" s="0" t="n">
+        <v>14.33</v>
+      </c>
+      <c r="E11" s="0" t="n">
+        <v>0.055</v>
+      </c>
+      <c r="F11" s="0" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="G11" s="0" t="n">
+        <v>0.057</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="B12" s="0" t="n">
+        <v>18.8</v>
+      </c>
+      <c r="C12" s="0" t="n">
+        <v>18.93</v>
+      </c>
+      <c r="D12" s="0" t="n">
+        <v>18.87</v>
+      </c>
+      <c r="E12" s="0" t="n">
+        <v>0.061</v>
+      </c>
+      <c r="F12" s="0" t="n">
+        <v>0.07</v>
+      </c>
+      <c r="G12" s="0" t="n">
+        <v>0.065</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="B13" s="0" t="n">
+        <v>18.53</v>
+      </c>
+      <c r="C13" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="D13" s="0" t="n">
+        <v>19.77</v>
+      </c>
+      <c r="E13" s="0" t="n">
+        <v>0.064</v>
+      </c>
+      <c r="F13" s="0" t="n">
+        <v>0.079</v>
+      </c>
+      <c r="G13" s="0" t="n">
+        <v>0.072</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="B14" s="0" t="n">
+        <v>18.93</v>
+      </c>
+      <c r="C14" s="0" t="n">
+        <v>20.73</v>
+      </c>
+      <c r="D14" s="0" t="n">
+        <v>19.83</v>
+      </c>
+      <c r="E14" s="0" t="n">
+        <v>0.069</v>
+      </c>
+      <c r="F14" s="0" t="n">
+        <v>0.079</v>
+      </c>
+      <c r="G14" s="0" t="n">
+        <v>0.074</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="B15" s="0" t="n">
+        <v>21.47</v>
+      </c>
+      <c r="C15" s="0" t="n">
+        <v>22.33</v>
+      </c>
+      <c r="D15" s="0" t="n">
+        <v>21.9</v>
+      </c>
+      <c r="E15" s="0" t="n">
+        <v>0.068</v>
+      </c>
+      <c r="F15" s="0" t="n">
+        <v>0.085</v>
+      </c>
+      <c r="G15" s="0" t="n">
+        <v>0.076</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="B16" s="0" t="n">
+        <v>20.87</v>
+      </c>
+      <c r="C16" s="0" t="n">
+        <v>24.33</v>
+      </c>
+      <c r="D16" s="0" t="n">
+        <v>22.6</v>
+      </c>
+      <c r="E16" s="0" t="n">
+        <v>0.074</v>
+      </c>
+      <c r="F16" s="0" t="n">
+        <v>0.087</v>
+      </c>
+      <c r="G16" s="0" t="n">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="B17" s="0" t="n">
+        <v>23.8</v>
+      </c>
+      <c r="C17" s="0" t="n">
+        <v>27.67</v>
+      </c>
+      <c r="D17" s="0" t="n">
+        <v>25.73</v>
+      </c>
+      <c r="E17" s="0" t="n">
+        <v>0.086</v>
+      </c>
+      <c r="F17" s="0" t="n">
+        <v>0.098</v>
+      </c>
+      <c r="G17" s="0" t="n">
+        <v>0.092</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="B18" s="0" t="n">
+        <v>24.67</v>
+      </c>
+      <c r="C18" s="0" t="n">
+        <v>28.2</v>
+      </c>
+      <c r="D18" s="0" t="n">
+        <v>26.43</v>
+      </c>
+      <c r="E18" s="0" t="n">
+        <v>0.073</v>
+      </c>
+      <c r="F18" s="0" t="n">
+        <v>0.098</v>
+      </c>
+      <c r="G18" s="0" t="n">
+        <v>0.085</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="B19" s="0" t="n">
+        <v>23.47</v>
+      </c>
+      <c r="C19" s="0" t="n">
+        <v>29.53</v>
+      </c>
+      <c r="D19" s="0" t="n">
+        <v>26.5</v>
+      </c>
+      <c r="E19" s="0" t="n">
+        <v>0.069</v>
+      </c>
+      <c r="F19" s="0" t="n">
+        <v>0.087</v>
+      </c>
+      <c r="G19" s="0" t="n">
+        <v>0.078</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B20" s="0" t="n">
+        <v>23.73</v>
+      </c>
+      <c r="C20" s="0" t="n">
+        <v>29.67</v>
+      </c>
+      <c r="D20" s="0" t="n">
+        <v>26.7</v>
+      </c>
+      <c r="E20" s="0" t="n">
+        <v>0.073</v>
+      </c>
+      <c r="F20" s="0" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="G20" s="0" t="n">
+        <v>0.087</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="B21" s="0" t="n">
+        <v>25.8</v>
+      </c>
+      <c r="C21" s="0" t="n">
+        <v>28.2</v>
+      </c>
+      <c r="D21" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="E21" s="0" t="n">
+        <v>0.105</v>
+      </c>
+      <c r="F21" s="0" t="n">
+        <v>0.112</v>
+      </c>
+      <c r="G21" s="0" t="n">
+        <v>0.109</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="B22" s="0" t="n">
+        <v>25.4</v>
+      </c>
+      <c r="C22" s="0" t="n">
+        <v>28.87</v>
+      </c>
+      <c r="D22" s="0" t="n">
+        <v>27.13</v>
+      </c>
+      <c r="E22" s="0" t="n">
+        <v>0.09</v>
+      </c>
+      <c r="F22" s="0" t="n">
+        <v>0.099</v>
+      </c>
+      <c r="G22" s="0" t="n">
+        <v>0.094</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="B23" s="0" t="n">
+        <v>28.33</v>
+      </c>
+      <c r="C23" s="0" t="n">
+        <v>26.13</v>
+      </c>
+      <c r="D23" s="0" t="n">
+        <v>27.23</v>
+      </c>
+      <c r="E23" s="0" t="n">
+        <v>0.081</v>
+      </c>
+      <c r="F23" s="0" t="n">
+        <v>0.079</v>
+      </c>
+      <c r="G23" s="0" t="n">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="B24" s="0" t="n">
+        <v>31.4</v>
+      </c>
+      <c r="C24" s="0" t="n">
+        <v>23.47</v>
+      </c>
+      <c r="D24" s="0" t="n">
+        <v>27.43</v>
+      </c>
+      <c r="E24" s="0" t="n">
+        <v>0.069</v>
+      </c>
+      <c r="F24" s="0" t="n">
+        <v>0.045</v>
+      </c>
+      <c r="G24" s="0" t="n">
+        <v>0.057</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="B25" s="0" t="n">
+        <v>24.53</v>
+      </c>
+      <c r="C25" s="0" t="n">
+        <v>30.4</v>
+      </c>
+      <c r="D25" s="0" t="n">
+        <v>27.47</v>
+      </c>
+      <c r="E25" s="0" t="n">
+        <v>0.087</v>
+      </c>
+      <c r="F25" s="0" t="n">
+        <v>0.148</v>
+      </c>
+      <c r="G25" s="0" t="n">
+        <v>0.118</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="B26" s="0" t="n">
+        <v>30.53</v>
+      </c>
+      <c r="C26" s="0" t="n">
+        <v>26.53</v>
+      </c>
+      <c r="D26" s="0" t="n">
+        <v>28.53</v>
+      </c>
+      <c r="E26" s="0" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F26" s="0" t="n">
+        <v>0.098</v>
+      </c>
+      <c r="G26" s="0" t="n">
+        <v>0.099</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="B27" s="0" t="n">
+        <v>26.87</v>
+      </c>
+      <c r="C27" s="0" t="n">
+        <v>31.4</v>
+      </c>
+      <c r="D27" s="0" t="n">
+        <v>29.13</v>
+      </c>
+      <c r="E27" s="0" t="n">
+        <v>0.111</v>
+      </c>
+      <c r="F27" s="0" t="n">
+        <v>0.146</v>
+      </c>
+      <c r="G27" s="0" t="n">
+        <v>0.129</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="B28" s="0" t="n">
+        <v>30.13</v>
+      </c>
+      <c r="C28" s="0" t="n">
+        <v>28.6</v>
+      </c>
+      <c r="D28" s="0" t="n">
+        <v>29.37</v>
+      </c>
+      <c r="E28" s="0" t="n">
+        <v>0.065</v>
+      </c>
+      <c r="F28" s="0" t="n">
+        <v>0.078</v>
+      </c>
+      <c r="G28" s="0" t="n">
+        <v>0.072</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="B29" s="0" t="n">
+        <v>29.93</v>
+      </c>
+      <c r="C29" s="0" t="n">
+        <v>29.6</v>
+      </c>
+      <c r="D29" s="0" t="n">
+        <v>29.77</v>
+      </c>
+      <c r="E29" s="0" t="n">
+        <v>0.068</v>
+      </c>
+      <c r="F29" s="0" t="n">
+        <v>0.088</v>
+      </c>
+      <c r="G29" s="0" t="n">
+        <v>0.078</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="B30" s="0" t="n">
+        <v>28.2</v>
+      </c>
+      <c r="C30" s="0" t="n">
+        <v>32.47</v>
+      </c>
+      <c r="D30" s="0" t="n">
+        <v>30.33</v>
+      </c>
+      <c r="E30" s="0" t="n">
+        <v>0.086</v>
+      </c>
+      <c r="F30" s="0" t="n">
+        <v>0.098</v>
+      </c>
+      <c r="G30" s="0" t="n">
+        <v>0.092</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="B31" s="0" t="n">
+        <v>28.67</v>
+      </c>
+      <c r="C31" s="0" t="n">
+        <v>32.2</v>
+      </c>
+      <c r="D31" s="0" t="n">
+        <v>30.43</v>
+      </c>
+      <c r="E31" s="0" t="n">
+        <v>0.102</v>
+      </c>
+      <c r="F31" s="0" t="n">
+        <v>0.113</v>
+      </c>
+      <c r="G31" s="0" t="n">
+        <v>0.107</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="B32" s="0" t="n">
+        <v>32.73</v>
+      </c>
+      <c r="C32" s="0" t="n">
+        <v>28.33</v>
+      </c>
+      <c r="D32" s="0" t="n">
+        <v>30.53</v>
+      </c>
+      <c r="E32" s="0" t="n">
+        <v>0.082</v>
+      </c>
+      <c r="F32" s="0" t="n">
+        <v>0.081</v>
+      </c>
+      <c r="G32" s="0" t="n">
+        <v>0.082</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="B33" s="0" t="n">
+        <v>33.6</v>
+      </c>
+      <c r="C33" s="0" t="n">
+        <v>28.13</v>
+      </c>
+      <c r="D33" s="0" t="n">
+        <v>30.87</v>
+      </c>
+      <c r="E33" s="0" t="n">
+        <v>0.07</v>
+      </c>
+      <c r="F33" s="0" t="n">
+        <v>0.089</v>
+      </c>
+      <c r="G33" s="0" t="n">
+        <v>0.079</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="B34" s="0" t="n">
+        <v>30.93</v>
+      </c>
+      <c r="C34" s="0" t="n">
+        <v>31.53</v>
+      </c>
+      <c r="D34" s="0" t="n">
+        <v>31.23</v>
+      </c>
+      <c r="E34" s="0" t="n">
+        <v>0.112</v>
+      </c>
+      <c r="F34" s="0" t="n">
+        <v>0.113</v>
+      </c>
+      <c r="G34" s="0" t="n">
+        <v>0.112</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="B35" s="0" t="n">
+        <v>31.6</v>
+      </c>
+      <c r="C35" s="0" t="n">
+        <v>30.93</v>
+      </c>
+      <c r="D35" s="0" t="n">
+        <v>31.27</v>
+      </c>
+      <c r="E35" s="0" t="n">
+        <v>0.102</v>
+      </c>
+      <c r="F35" s="0" t="n">
+        <v>0.105</v>
+      </c>
+      <c r="G35" s="0" t="n">
+        <v>0.103</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="B36" s="0" t="n">
+        <v>28.4</v>
+      </c>
+      <c r="C36" s="0" t="n">
+        <v>34.87</v>
+      </c>
+      <c r="D36" s="0" t="n">
+        <v>31.63</v>
+      </c>
+      <c r="E36" s="0" t="n">
+        <v>0.123</v>
+      </c>
+      <c r="F36" s="0" t="n">
+        <v>0.137</v>
+      </c>
+      <c r="G36" s="0" t="n">
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="B37" s="0" t="n">
+        <v>35.73</v>
+      </c>
+      <c r="C37" s="0" t="n">
+        <v>28.47</v>
+      </c>
+      <c r="D37" s="0" t="n">
+        <v>32.1</v>
+      </c>
+      <c r="E37" s="0" t="n">
+        <v>0.191</v>
+      </c>
+      <c r="F37" s="0" t="n">
+        <v>0.093</v>
+      </c>
+      <c r="G37" s="0" t="n">
+        <v>0.142</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="25" t="s">
+        <v>68</v>
+      </c>
+      <c r="B38" s="0" t="n">
+        <v>31.13</v>
+      </c>
+      <c r="C38" s="0" t="n">
+        <v>33.6</v>
+      </c>
+      <c r="D38" s="0" t="n">
+        <v>32.37</v>
+      </c>
+      <c r="E38" s="0" t="n">
+        <v>0.141</v>
+      </c>
+      <c r="F38" s="0" t="n">
+        <v>0.119</v>
+      </c>
+      <c r="G38" s="0" t="n">
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="B39" s="0" t="n">
+        <v>34.4</v>
+      </c>
+      <c r="C39" s="0" t="n">
+        <v>35.27</v>
+      </c>
+      <c r="D39" s="0" t="n">
+        <v>34.83</v>
+      </c>
+      <c r="E39" s="0" t="n">
+        <v>0.125</v>
+      </c>
+      <c r="F39" s="0" t="n">
+        <v>0.128</v>
+      </c>
+      <c r="G39" s="0" t="n">
+        <v>0.127</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="B40" s="0" t="n">
+        <v>38.2</v>
+      </c>
+      <c r="C40" s="0" t="n">
+        <v>35.67</v>
+      </c>
+      <c r="D40" s="0" t="n">
+        <v>36.93</v>
+      </c>
+      <c r="E40" s="0" t="n">
+        <v>0.102</v>
+      </c>
+      <c r="F40" s="0" t="n">
+        <v>0.119</v>
+      </c>
+      <c r="G40" s="0" t="n">
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="B41" s="0" t="n">
+        <v>38.2</v>
+      </c>
+      <c r="C41" s="0" t="n">
+        <v>35.67</v>
+      </c>
+      <c r="D41" s="0" t="n">
+        <v>36.93</v>
+      </c>
+      <c r="E41" s="0" t="n">
+        <v>0.102</v>
+      </c>
+      <c r="F41" s="0" t="n">
+        <v>0.119</v>
+      </c>
+      <c r="G41" s="0" t="n">
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="B42" s="0" t="n">
+        <v>41.47</v>
+      </c>
+      <c r="C42" s="0" t="n">
+        <v>32.53</v>
+      </c>
+      <c r="D42" s="0" t="n">
+        <v>37</v>
+      </c>
+      <c r="E42" s="0" t="n">
+        <v>0.288</v>
+      </c>
+      <c r="F42" s="0" t="n">
+        <v>0.099</v>
+      </c>
+      <c r="G42" s="0" t="n">
+        <v>0.194</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="B43" s="0" t="n">
+        <v>33.4</v>
+      </c>
+      <c r="C43" s="0" t="n">
+        <v>40.8</v>
+      </c>
+      <c r="D43" s="0" t="n">
+        <v>37.1</v>
+      </c>
+      <c r="E43" s="0" t="n">
+        <v>0.084</v>
+      </c>
+      <c r="F43" s="0" t="n">
+        <v>0.122</v>
+      </c>
+      <c r="G43" s="0" t="n">
+        <v>0.103</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="B44" s="0" t="n">
+        <v>35.73</v>
+      </c>
+      <c r="C44" s="0" t="n">
+        <v>38.6</v>
+      </c>
+      <c r="D44" s="0" t="n">
+        <v>37.17</v>
+      </c>
+      <c r="E44" s="0" t="n">
+        <v>0.112</v>
+      </c>
+      <c r="F44" s="0" t="n">
+        <v>0.229</v>
+      </c>
+      <c r="G44" s="0" t="n">
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="B45" s="0" t="n">
+        <v>35.73</v>
+      </c>
+      <c r="C45" s="0" t="n">
+        <v>38.73</v>
+      </c>
+      <c r="D45" s="0" t="n">
+        <v>37.23</v>
+      </c>
+      <c r="E45" s="0" t="n">
+        <v>0.172</v>
+      </c>
+      <c r="F45" s="0" t="n">
+        <v>0.235</v>
+      </c>
+      <c r="G45" s="0" t="n">
+        <v>0.204</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="B46" s="0" t="n">
+        <v>42.27</v>
+      </c>
+      <c r="C46" s="0" t="n">
+        <v>38.53</v>
+      </c>
+      <c r="D46" s="0" t="n">
+        <v>40.4</v>
+      </c>
+      <c r="E46" s="0" t="n">
+        <v>0.098</v>
+      </c>
+      <c r="F46" s="0" t="n">
+        <v>0.118</v>
+      </c>
+      <c r="G46" s="0" t="n">
+        <v>0.108</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="B47" s="0" t="n">
+        <v>41.87</v>
+      </c>
+      <c r="C47" s="0" t="n">
+        <v>39.47</v>
+      </c>
+      <c r="D47" s="0" t="n">
+        <v>40.67</v>
+      </c>
+      <c r="E47" s="0" t="n">
+        <v>0.102</v>
+      </c>
+      <c r="F47" s="0" t="n">
+        <v>0.136</v>
+      </c>
+      <c r="G47" s="0" t="n">
+        <v>0.119</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="B48" s="0" t="n">
+        <v>40.27</v>
+      </c>
+      <c r="C48" s="0" t="n">
+        <v>44.27</v>
+      </c>
+      <c r="D48" s="0" t="n">
+        <v>42.27</v>
+      </c>
+      <c r="E48" s="0" t="n">
+        <v>0.168</v>
+      </c>
+      <c r="F48" s="0" t="n">
+        <v>0.18</v>
+      </c>
+      <c r="G48" s="0" t="n">
+        <v>0.174</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="B49" s="0" t="n">
+        <v>40.93</v>
+      </c>
+      <c r="C49" s="0" t="n">
+        <v>44.07</v>
+      </c>
+      <c r="D49" s="0" t="n">
+        <v>42.5</v>
+      </c>
+      <c r="E49" s="0" t="n">
+        <v>0.17</v>
+      </c>
+      <c r="F49" s="0" t="n">
+        <v>0.181</v>
+      </c>
+      <c r="G49" s="0" t="n">
+        <v>0.175</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="B50" s="0" t="n">
+        <v>44.33</v>
+      </c>
+      <c r="C50" s="0" t="n">
+        <v>41.93</v>
+      </c>
+      <c r="D50" s="0" t="n">
+        <v>43.13</v>
+      </c>
+      <c r="E50" s="0" t="n">
+        <v>0.111</v>
+      </c>
+      <c r="F50" s="0" t="n">
+        <v>0.144</v>
+      </c>
+      <c r="G50" s="0" t="n">
+        <v>0.127</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="25" t="s">
+        <v>80</v>
+      </c>
+      <c r="B51" s="0" t="n">
+        <v>42.87</v>
+      </c>
+      <c r="C51" s="0" t="n">
+        <v>43.47</v>
+      </c>
+      <c r="D51" s="0" t="n">
+        <v>43.17</v>
+      </c>
+      <c r="E51" s="0" t="n">
+        <v>0.19</v>
+      </c>
+      <c r="F51" s="0" t="n">
+        <v>0.194</v>
+      </c>
+      <c r="G51" s="0" t="n">
+        <v>0.192</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="B52" s="0" t="n">
+        <v>41</v>
+      </c>
+      <c r="C52" s="0" t="n">
+        <v>46</v>
+      </c>
+      <c r="D52" s="0" t="n">
+        <v>43.5</v>
+      </c>
+      <c r="E52" s="0" t="n">
+        <v>0.199</v>
+      </c>
+      <c r="F52" s="0" t="n">
+        <v>0.244</v>
+      </c>
+      <c r="G52" s="0" t="n">
+        <v>0.221</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="B53" s="0" t="n">
+        <v>44.93</v>
+      </c>
+      <c r="C53" s="0" t="n">
+        <v>48.47</v>
+      </c>
+      <c r="D53" s="0" t="n">
+        <v>46.7</v>
+      </c>
+      <c r="E53" s="0" t="n">
+        <v>0.224</v>
+      </c>
+      <c r="F53" s="0" t="n">
+        <v>0.267</v>
+      </c>
+      <c r="G53" s="0" t="n">
+        <v>0.245</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="B54" s="0" t="n">
+        <v>46.8</v>
+      </c>
+      <c r="C54" s="0" t="n">
+        <v>47.87</v>
+      </c>
+      <c r="D54" s="0" t="n">
+        <v>47.33</v>
+      </c>
+      <c r="E54" s="0" t="n">
+        <v>0.212</v>
+      </c>
+      <c r="F54" s="0" t="n">
+        <v>0.204</v>
+      </c>
+      <c r="G54" s="0" t="n">
+        <v>0.208</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="B55" s="0" t="n">
+        <v>47.2</v>
+      </c>
+      <c r="C55" s="0" t="n">
+        <v>48.67</v>
+      </c>
+      <c r="D55" s="0" t="n">
+        <v>47.93</v>
+      </c>
+      <c r="E55" s="0" t="n">
+        <v>0.224</v>
+      </c>
+      <c r="F55" s="0" t="n">
+        <v>0.237</v>
+      </c>
+      <c r="G55" s="0" t="n">
+        <v>0.23</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="24" t="s">
+        <v>85</v>
+      </c>
+      <c r="B56" s="0" t="n">
+        <v>47.27</v>
+      </c>
+      <c r="C56" s="0" t="n">
+        <v>48.73</v>
+      </c>
+      <c r="D56" s="0" t="n">
+        <v>48</v>
+      </c>
+      <c r="E56" s="0" t="n">
+        <v>0.224</v>
+      </c>
+      <c r="F56" s="0" t="n">
+        <v>0.237</v>
+      </c>
+      <c r="G56" s="0" t="n">
+        <v>0.23</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="B57" s="0" t="n">
+        <v>48.93</v>
+      </c>
+      <c r="C57" s="0" t="n">
+        <v>51.6</v>
+      </c>
+      <c r="D57" s="0" t="n">
+        <v>50.27</v>
+      </c>
+      <c r="E57" s="0" t="n">
+        <v>0.253</v>
+      </c>
+      <c r="F57" s="0" t="n">
+        <v>0.238</v>
+      </c>
+      <c r="G57" s="0" t="n">
+        <v>0.245</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="B58" s="0" t="n">
+        <v>52.73</v>
+      </c>
+      <c r="C58" s="0" t="n">
+        <v>52.8</v>
+      </c>
+      <c r="D58" s="0" t="n">
+        <v>52.77</v>
+      </c>
+      <c r="E58" s="0" t="n">
+        <v>0.24</v>
+      </c>
+      <c r="F58" s="0" t="n">
+        <v>0.254</v>
+      </c>
+      <c r="G58" s="0" t="n">
+        <v>0.247</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="B59" s="0" t="n">
+        <v>50.67</v>
+      </c>
+      <c r="C59" s="0" t="n">
+        <v>55.2</v>
+      </c>
+      <c r="D59" s="0" t="n">
+        <v>52.93</v>
+      </c>
+      <c r="E59" s="0" t="n">
+        <v>0.353</v>
+      </c>
+      <c r="F59" s="0" t="n">
+        <v>0.465</v>
+      </c>
+      <c r="G59" s="0" t="n">
+        <v>0.409</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="B60" s="0" t="n">
+        <v>55.93</v>
+      </c>
+      <c r="C60" s="0" t="n">
+        <v>51.93</v>
+      </c>
+      <c r="D60" s="0" t="n">
+        <v>53.93</v>
+      </c>
+      <c r="E60" s="0" t="n">
+        <v>0.385</v>
+      </c>
+      <c r="F60" s="0" t="n">
+        <v>0.467</v>
+      </c>
+      <c r="G60" s="0" t="n">
+        <v>0.426</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="B61" s="0" t="n">
+        <v>58.67</v>
+      </c>
+      <c r="C61" s="0" t="n">
+        <v>49.33</v>
+      </c>
+      <c r="D61" s="0" t="n">
+        <v>54</v>
+      </c>
+      <c r="E61" s="0" t="n">
+        <v>0.673</v>
+      </c>
+      <c r="F61" s="0" t="n">
+        <v>0.237</v>
+      </c>
+      <c r="G61" s="0" t="n">
+        <v>0.455</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="B62" s="0" t="n">
+        <v>59</v>
+      </c>
+      <c r="C62" s="0" t="n">
+        <v>56.73</v>
+      </c>
+      <c r="D62" s="0" t="n">
+        <v>57.87</v>
+      </c>
+      <c r="E62" s="0" t="n">
+        <v>0.619</v>
+      </c>
+      <c r="F62" s="0" t="n">
+        <v>0.836</v>
+      </c>
+      <c r="G62" s="0" t="n">
+        <v>0.728</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="B63" s="0" t="n">
+        <v>61.87</v>
+      </c>
+      <c r="C63" s="0" t="n">
+        <v>58.27</v>
+      </c>
+      <c r="D63" s="0" t="n">
+        <v>60.07</v>
+      </c>
+      <c r="E63" s="0" t="n">
+        <v>0.715</v>
+      </c>
+      <c r="F63" s="0" t="n">
+        <v>0.99</v>
+      </c>
+      <c r="G63" s="0" t="n">
+        <v>0.852</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="B64" s="0" t="n">
+        <v>65.13</v>
+      </c>
+      <c r="C64" s="0" t="n">
+        <v>60.8</v>
+      </c>
+      <c r="D64" s="0" t="n">
+        <v>62.97</v>
+      </c>
+      <c r="E64" s="0" t="n">
+        <v>0.844</v>
+      </c>
+      <c r="F64" s="0" t="n">
+        <v>1.164</v>
+      </c>
+      <c r="G64" s="0" t="n">
+        <v>1.004</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="B65" s="0" t="n">
+        <v>65</v>
+      </c>
+      <c r="C65" s="0" t="n">
+        <v>61.47</v>
+      </c>
+      <c r="D65" s="0" t="n">
+        <v>63.23</v>
+      </c>
+      <c r="E65" s="0" t="n">
+        <v>0.897</v>
+      </c>
+      <c r="F65" s="0" t="n">
+        <v>1.067</v>
+      </c>
+      <c r="G65" s="0" t="n">
+        <v>0.982</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="B66" s="0" t="n">
+        <v>66.53</v>
+      </c>
+      <c r="C66" s="0" t="n">
+        <v>60.33</v>
+      </c>
+      <c r="D66" s="0" t="n">
+        <v>63.43</v>
+      </c>
+      <c r="E66" s="0" t="n">
+        <v>0.497</v>
+      </c>
+      <c r="F66" s="0" t="n">
+        <v>0.553</v>
+      </c>
+      <c r="G66" s="0" t="n">
+        <v>0.525</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="B67" s="0" t="n">
+        <v>63.07</v>
+      </c>
+      <c r="C67" s="0" t="n">
+        <v>65.27</v>
+      </c>
+      <c r="D67" s="0" t="n">
+        <v>64.17</v>
+      </c>
+      <c r="E67" s="0" t="n">
+        <v>0.438</v>
+      </c>
+      <c r="F67" s="0" t="n">
+        <v>0.596</v>
+      </c>
+      <c r="G67" s="0" t="n">
+        <v>0.517</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="B68" s="0" t="n">
+        <v>64.8</v>
+      </c>
+      <c r="C68" s="0" t="n">
+        <v>65.8</v>
+      </c>
+      <c r="D68" s="0" t="n">
+        <v>65.3</v>
+      </c>
+      <c r="E68" s="0" t="n">
+        <v>0.883</v>
+      </c>
+      <c r="F68" s="0" t="n">
+        <v>1.22</v>
+      </c>
+      <c r="G68" s="0" t="n">
+        <v>1.051</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="B69" s="0" t="n">
+        <v>68.13</v>
+      </c>
+      <c r="C69" s="0" t="n">
+        <v>62.73</v>
+      </c>
+      <c r="D69" s="0" t="n">
+        <v>65.43</v>
+      </c>
+      <c r="E69" s="0" t="n">
+        <v>0.935</v>
+      </c>
+      <c r="F69" s="0" t="n">
+        <v>1.29</v>
+      </c>
+      <c r="G69" s="0" t="n">
+        <v>1.113</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="B70" s="0" t="n">
+        <v>59.93</v>
+      </c>
+      <c r="C70" s="0" t="n">
+        <v>71.73</v>
+      </c>
+      <c r="D70" s="0" t="n">
+        <v>65.83</v>
+      </c>
+      <c r="E70" s="0" t="n">
+        <v>28627.758</v>
+      </c>
+      <c r="F70" s="0" t="n">
+        <v>1174.168</v>
+      </c>
+      <c r="G70" s="0" t="n">
+        <v>14900.963</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="B71" s="0" t="n">
+        <v>65.73</v>
+      </c>
+      <c r="C71" s="0" t="n">
+        <v>67.2</v>
+      </c>
+      <c r="D71" s="0" t="n">
+        <v>66.47</v>
+      </c>
+      <c r="E71" s="0" t="n">
+        <v>0.763</v>
+      </c>
+      <c r="F71" s="0" t="n">
+        <v>1.329</v>
+      </c>
+      <c r="G71" s="0" t="n">
+        <v>1.046</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="B72" s="0" t="n">
+        <v>67.47</v>
+      </c>
+      <c r="C72" s="0" t="n">
+        <v>65.73</v>
+      </c>
+      <c r="D72" s="0" t="n">
+        <v>66.6</v>
+      </c>
+      <c r="E72" s="0" t="n">
+        <v>0.947</v>
+      </c>
+      <c r="F72" s="0" t="n">
+        <v>1.295</v>
+      </c>
+      <c r="G72" s="0" t="n">
+        <v>1.121</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="B73" s="0" t="n">
+        <v>67.87</v>
+      </c>
+      <c r="C73" s="0" t="n">
+        <v>73.07</v>
+      </c>
+      <c r="D73" s="0" t="n">
+        <v>70.47</v>
+      </c>
+      <c r="E73" s="0" t="n">
+        <v>0.772</v>
+      </c>
+      <c r="F73" s="0" t="n">
+        <v>1.088</v>
+      </c>
+      <c r="G73" s="0" t="n">
+        <v>0.93</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="B74" s="0" t="n">
+        <v>72.53</v>
+      </c>
+      <c r="C74" s="0" t="n">
+        <v>68.87</v>
+      </c>
+      <c r="D74" s="0" t="n">
+        <v>70.7</v>
+      </c>
+      <c r="E74" s="0" t="n">
+        <v>1.017</v>
+      </c>
+      <c r="F74" s="0" t="n">
+        <v>1.429</v>
+      </c>
+      <c r="G74" s="0" t="n">
+        <v>1.223</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="B75" s="0" t="n">
+        <v>71.33</v>
+      </c>
+      <c r="C75" s="0" t="n">
+        <v>71.4</v>
+      </c>
+      <c r="D75" s="0" t="n">
+        <v>71.37</v>
+      </c>
+      <c r="E75" s="0" t="n">
+        <v>0.707</v>
+      </c>
+      <c r="F75" s="0" t="n">
+        <v>0.927</v>
+      </c>
+      <c r="G75" s="0" t="n">
+        <v>0.817</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="B76" s="0" t="n">
+        <v>73</v>
+      </c>
+      <c r="C76" s="0" t="n">
+        <v>70.4</v>
+      </c>
+      <c r="D76" s="0" t="n">
+        <v>71.7</v>
+      </c>
+      <c r="E76" s="0" t="n">
+        <v>1.099</v>
+      </c>
+      <c r="F76" s="0" t="n">
+        <v>1.515</v>
+      </c>
+      <c r="G76" s="0" t="n">
+        <v>1.307</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="B77" s="0" t="n">
+        <v>73.27</v>
+      </c>
+      <c r="C77" s="0" t="n">
+        <v>72.27</v>
+      </c>
+      <c r="D77" s="0" t="n">
+        <v>72.77</v>
+      </c>
+      <c r="E77" s="0" t="n">
+        <v>1.103</v>
+      </c>
+      <c r="F77" s="0" t="n">
+        <v>1.523</v>
+      </c>
+      <c r="G77" s="0" t="n">
+        <v>1.313</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="B78" s="0" t="n">
+        <v>73.27</v>
+      </c>
+      <c r="C78" s="0" t="n">
+        <v>72.27</v>
+      </c>
+      <c r="D78" s="0" t="n">
+        <v>72.77</v>
+      </c>
+      <c r="E78" s="0" t="n">
+        <v>1.103</v>
+      </c>
+      <c r="F78" s="0" t="n">
+        <v>1.523</v>
+      </c>
+      <c r="G78" s="0" t="n">
+        <v>1.313</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="B79" s="0" t="n">
+        <v>73.27</v>
+      </c>
+      <c r="C79" s="0" t="n">
+        <v>72.27</v>
+      </c>
+      <c r="D79" s="0" t="n">
+        <v>72.77</v>
+      </c>
+      <c r="E79" s="0" t="n">
+        <v>1.103</v>
+      </c>
+      <c r="F79" s="0" t="n">
+        <v>1.523</v>
+      </c>
+      <c r="G79" s="0" t="n">
+        <v>1.313</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="B80" s="0" t="n">
+        <v>76.4</v>
+      </c>
+      <c r="C80" s="0" t="n">
+        <v>73.93</v>
+      </c>
+      <c r="D80" s="0" t="n">
+        <v>75.17</v>
+      </c>
+      <c r="E80" s="0" t="n">
+        <v>1.209</v>
+      </c>
+      <c r="F80" s="0" t="n">
+        <v>1.672</v>
+      </c>
+      <c r="G80" s="0" t="n">
+        <v>1.441</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="B81" s="0" t="n">
+        <v>76.87</v>
+      </c>
+      <c r="C81" s="0" t="n">
+        <v>74.53</v>
+      </c>
+      <c r="D81" s="0" t="n">
+        <v>75.7</v>
+      </c>
+      <c r="E81" s="0" t="n">
+        <v>1.209</v>
+      </c>
+      <c r="F81" s="0" t="n">
+        <v>1.675</v>
+      </c>
+      <c r="G81" s="0" t="n">
+        <v>1.442</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="B82" s="0" t="n">
+        <v>75.8</v>
+      </c>
+      <c r="C82" s="0" t="n">
+        <v>75.67</v>
+      </c>
+      <c r="D82" s="0" t="n">
+        <v>75.73</v>
+      </c>
+      <c r="E82" s="0" t="n">
+        <v>1.16</v>
+      </c>
+      <c r="F82" s="0" t="n">
+        <v>1.648</v>
+      </c>
+      <c r="G82" s="0" t="n">
+        <v>1.404</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="B83" s="0" t="n">
+        <v>73.73</v>
+      </c>
+      <c r="C83" s="0" t="n">
+        <v>77.8</v>
+      </c>
+      <c r="D83" s="0" t="n">
+        <v>75.77</v>
+      </c>
+      <c r="E83" s="0" t="n">
+        <v>0.948</v>
+      </c>
+      <c r="F83" s="0" t="n">
+        <v>1.428</v>
+      </c>
+      <c r="G83" s="0" t="n">
+        <v>1.188</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="B84" s="0" t="n">
+        <v>77.33</v>
+      </c>
+      <c r="C84" s="0" t="n">
+        <v>74.27</v>
+      </c>
+      <c r="D84" s="0" t="n">
+        <v>75.8</v>
+      </c>
+      <c r="E84" s="0" t="n">
+        <v>1.208</v>
+      </c>
+      <c r="F84" s="0" t="n">
+        <v>1.598</v>
+      </c>
+      <c r="G84" s="0" t="n">
+        <v>1.403</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="B85" s="0" t="n">
+        <v>76.13</v>
+      </c>
+      <c r="C85" s="0" t="n">
+        <v>75.6</v>
+      </c>
+      <c r="D85" s="0" t="n">
+        <v>75.87</v>
+      </c>
+      <c r="E85" s="0" t="n">
+        <v>1.086</v>
+      </c>
+      <c r="F85" s="0" t="n">
+        <v>1.514</v>
+      </c>
+      <c r="G85" s="0" t="n">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="B86" s="0" t="n">
+        <v>76.13</v>
+      </c>
+      <c r="C86" s="0" t="n">
+        <v>75.6</v>
+      </c>
+      <c r="D86" s="0" t="n">
+        <v>75.87</v>
+      </c>
+      <c r="E86" s="0" t="n">
+        <v>1.086</v>
+      </c>
+      <c r="F86" s="0" t="n">
+        <v>1.514</v>
+      </c>
+      <c r="G86" s="0" t="n">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="B87" s="0" t="n">
+        <v>76.4</v>
+      </c>
+      <c r="C87" s="0" t="n">
+        <v>79.47</v>
+      </c>
+      <c r="D87" s="0" t="n">
+        <v>77.93</v>
+      </c>
+      <c r="E87" s="0" t="n">
+        <v>1.115</v>
+      </c>
+      <c r="F87" s="0" t="n">
+        <v>1.625</v>
+      </c>
+      <c r="G87" s="0" t="n">
+        <v>1.37</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="B88" s="0" t="n">
+        <v>79.67</v>
+      </c>
+      <c r="C88" s="0" t="n">
+        <v>78.33</v>
+      </c>
+      <c r="D88" s="0" t="n">
+        <v>79</v>
+      </c>
+      <c r="E88" s="0" t="n">
+        <v>1.157</v>
+      </c>
+      <c r="F88" s="0" t="n">
+        <v>1.571</v>
+      </c>
+      <c r="G88" s="0" t="n">
+        <v>1.364</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="B89" s="0" t="n">
+        <v>79.4</v>
+      </c>
+      <c r="C89" s="0" t="n">
+        <v>78.93</v>
+      </c>
+      <c r="D89" s="0" t="n">
+        <v>79.17</v>
+      </c>
+      <c r="E89" s="0" t="n">
+        <v>1.137</v>
+      </c>
+      <c r="F89" s="0" t="n">
+        <v>1.506</v>
+      </c>
+      <c r="G89" s="0" t="n">
+        <v>1.321</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="B90" s="0" t="n">
+        <v>80.6</v>
+      </c>
+      <c r="C90" s="0" t="n">
+        <v>80</v>
+      </c>
+      <c r="D90" s="0" t="n">
+        <v>80.3</v>
+      </c>
+      <c r="E90" s="0" t="n">
+        <v>2.857</v>
+      </c>
+      <c r="F90" s="0" t="n">
+        <v>2.463</v>
+      </c>
+      <c r="G90" s="0" t="n">
+        <v>2.66</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="B91" s="0" t="n">
+        <v>80.6</v>
+      </c>
+      <c r="C91" s="0" t="n">
+        <v>80</v>
+      </c>
+      <c r="D91" s="0" t="n">
+        <v>80.3</v>
+      </c>
+      <c r="E91" s="0" t="n">
+        <v>2.857</v>
+      </c>
+      <c r="F91" s="0" t="n">
+        <v>2.463</v>
+      </c>
+      <c r="G91" s="0" t="n">
+        <v>2.66</v>
+      </c>
+    </row>
+    <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="B92" s="0" t="n">
+        <v>78.93</v>
+      </c>
+      <c r="C92" s="0" t="n">
+        <v>81.87</v>
+      </c>
+      <c r="D92" s="0" t="n">
+        <v>80.4</v>
+      </c>
+      <c r="E92" s="0" t="n">
+        <v>1.092</v>
+      </c>
+      <c r="F92" s="0" t="n">
+        <v>1.569</v>
+      </c>
+      <c r="G92" s="0" t="n">
+        <v>1.33</v>
+      </c>
+    </row>
+    <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A93" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="B93" s="0" t="n">
+        <v>82.2</v>
+      </c>
+      <c r="C93" s="0" t="n">
+        <v>82.53</v>
+      </c>
+      <c r="D93" s="0" t="n">
+        <v>82.37</v>
+      </c>
+      <c r="E93" s="0" t="n">
+        <v>1.246</v>
+      </c>
+      <c r="F93" s="0" t="n">
+        <v>1.73</v>
+      </c>
+      <c r="G93" s="0" t="n">
+        <v>1.488</v>
+      </c>
+    </row>
+    <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="B94" s="0" t="n">
+        <v>83.4</v>
+      </c>
+      <c r="C94" s="0" t="n">
+        <v>82.47</v>
+      </c>
+      <c r="D94" s="0" t="n">
+        <v>82.93</v>
+      </c>
+      <c r="E94" s="0" t="n">
+        <v>1.426</v>
+      </c>
+      <c r="F94" s="0" t="n">
+        <v>1.728</v>
+      </c>
+      <c r="G94" s="0" t="n">
+        <v>1.577</v>
+      </c>
+    </row>
+    <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A95" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="B95" s="0" t="n">
+        <v>85.13</v>
+      </c>
+      <c r="C95" s="0" t="n">
+        <v>85.73</v>
+      </c>
+      <c r="D95" s="0" t="n">
+        <v>85.43</v>
+      </c>
+      <c r="E95" s="0" t="n">
+        <v>1.285</v>
+      </c>
+      <c r="F95" s="0" t="n">
+        <v>1.769</v>
+      </c>
+      <c r="G95" s="0" t="n">
+        <v>1.527</v>
+      </c>
+    </row>
+    <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A96" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="B96" s="0" t="n">
+        <v>86.73</v>
+      </c>
+      <c r="C96" s="0" t="n">
+        <v>87.53</v>
+      </c>
+      <c r="D96" s="0" t="n">
+        <v>87.13</v>
+      </c>
+      <c r="E96" s="0" t="n">
+        <v>1.303</v>
+      </c>
+      <c r="F96" s="0" t="n">
+        <v>1.793</v>
+      </c>
+      <c r="G96" s="0" t="n">
+        <v>1.548</v>
+      </c>
+    </row>
+    <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A97" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="B97" s="0" t="n">
+        <v>86.6</v>
+      </c>
+      <c r="C97" s="0" t="n">
+        <v>88.67</v>
+      </c>
+      <c r="D97" s="0" t="n">
+        <v>87.63</v>
+      </c>
+      <c r="E97" s="0" t="n">
+        <v>1.321</v>
+      </c>
+      <c r="F97" s="0" t="n">
+        <v>1.851</v>
+      </c>
+      <c r="G97" s="0" t="n">
+        <v>1.586</v>
+      </c>
+    </row>
+    <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A98" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="B98" s="0" t="n">
+        <v>88.53</v>
+      </c>
+      <c r="C98" s="0" t="n">
+        <v>88.73</v>
+      </c>
+      <c r="D98" s="0" t="n">
+        <v>88.63</v>
+      </c>
+      <c r="E98" s="0" t="n">
+        <v>1.774</v>
+      </c>
+      <c r="F98" s="0" t="n">
+        <v>2.43</v>
+      </c>
+      <c r="G98" s="0" t="n">
+        <v>2.102</v>
+      </c>
+    </row>
+    <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A99" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="B99" s="0" t="n">
+        <v>90.47</v>
+      </c>
+      <c r="C99" s="0" t="n">
+        <v>90.93</v>
+      </c>
+      <c r="D99" s="0" t="n">
+        <v>90.7</v>
+      </c>
+      <c r="E99" s="0" t="n">
+        <v>1.717</v>
+      </c>
+      <c r="F99" s="0" t="n">
+        <v>2.444</v>
+      </c>
+      <c r="G99" s="0" t="n">
+        <v>2.08</v>
+      </c>
+    </row>
+    <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A100" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="B100" s="0" t="n">
+        <v>90.47</v>
+      </c>
+      <c r="C100" s="0" t="n">
+        <v>90.93</v>
+      </c>
+      <c r="D100" s="0" t="n">
+        <v>90.7</v>
+      </c>
+      <c r="E100" s="0" t="n">
+        <v>1.717</v>
+      </c>
+      <c r="F100" s="0" t="n">
+        <v>2.444</v>
+      </c>
+      <c r="G100" s="0" t="n">
+        <v>2.08</v>
+      </c>
+    </row>
+    <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A101" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="B101" s="0" t="n">
+        <v>92</v>
+      </c>
+      <c r="C101" s="0" t="n">
+        <v>93</v>
+      </c>
+      <c r="D101" s="0" t="n">
+        <v>92.67</v>
+      </c>
+      <c r="E101" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="F101" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="G101" s="0" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A102" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="B102" s="0" t="n">
+        <v>92.67</v>
+      </c>
+      <c r="C102" s="0" t="n">
+        <v>93</v>
+      </c>
+      <c r="D102" s="0" t="n">
+        <v>92.75</v>
+      </c>
+      <c r="E102" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="F102" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="G102" s="0" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A103" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="B103" s="0" t="n">
+        <v>93</v>
+      </c>
+      <c r="C103" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="D103" s="0" t="n">
+        <v>93</v>
+      </c>
+      <c r="E103" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="F103" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="G103" s="0" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A104" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="B104" s="0" t="n">
+        <v>93</v>
+      </c>
+      <c r="C104" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="D104" s="0" t="n">
+        <v>93</v>
+      </c>
+      <c r="E104" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="F104" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="G104" s="0" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A105" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="B105" s="0" t="n">
+        <v>93</v>
+      </c>
+      <c r="C105" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="D105" s="0" t="n">
+        <v>93</v>
+      </c>
+      <c r="E105" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="F105" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="G105" s="0" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A106" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="B106" s="0" t="n">
+        <v>93</v>
+      </c>
+      <c r="C106" s="0" t="n">
+        <v>93</v>
+      </c>
+      <c r="D106" s="0" t="n">
+        <v>93</v>
+      </c>
+      <c r="E106" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="F106" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="G106" s="0" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A107" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="B107" s="0" t="n">
+        <v>93</v>
+      </c>
+      <c r="C107" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="D107" s="0" t="n">
+        <v>93</v>
+      </c>
+      <c r="E107" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="F107" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="G107" s="0" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A108" s="0" t="s">
+        <v>132</v>
+      </c>
+      <c r="B108" s="0" t="n">
+        <v>93</v>
+      </c>
+      <c r="C108" s="0" t="n">
+        <v>93</v>
+      </c>
+      <c r="D108" s="0" t="n">
+        <v>93</v>
+      </c>
+      <c r="E108" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="F108" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="G108" s="0" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A109" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="B109" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="C109" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="D109" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="E109" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="F109" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="G109" s="0" t="s">
+        <v>129</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>